<commit_message>
improved comments but still not correct noise rate added args to moving_dot.py to enable setting # cycles etc from command line fixed bug in emulator.py to add noise only after initial noiseless frame initializes lowpass filter.
</commit_message>
<xml_diff>
--- a/media/noise_event_rate_simulation.xlsx
+++ b/media/noise_event_rate_simulation.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tobi\Dropbox (Personal)\GitHub\SensorsINI\v2e\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE4461C-6F0D-4053-9C48-A900CACC3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1E474E-F736-4831-9243-C3A028AC1A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="720" windowWidth="25950" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="720" windowWidth="37890" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="noise_event_rate_simulation" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,13 +31,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tobi Delbruck</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3FB7CFAE-F393-41B6-941F-04D2E509F49C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tobi Delbruck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+for 1kHz f3db bandwidth</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>thresh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      on_event_rate</t>
   </si>
   <si>
     <t>log10_thr</t>
@@ -46,12 +76,30 @@
   <si>
     <t>log10_rate</t>
   </si>
+  <si>
+    <t>thr/vn</t>
+  </si>
+  <si>
+    <t>vn/thr</t>
+  </si>
+  <si>
+    <t>vnthr0p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      on_event_rate_1khz</t>
+  </si>
+  <si>
+    <t>log10_rate_per_hz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +230,42 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -528,9 +612,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -660,7 +750,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.7361125909325428E-2"/>
+          <c:y val="9.0249915107210282E-2"/>
+          <c:w val="0.88926407654968931"/>
+          <c:h val="0.88942935058174077"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -673,7 +773,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>log10_rate</c:v>
+                  <c:v>log10_rate_per_hz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -764,7 +864,7 @@
             <c:numRef>
               <c:f>noise_event_rate_simulation!$C$2:$C$57</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
                   <c:v>-2.0852338630741474</c:v>
@@ -941,175 +1041,175 @@
             <c:numRef>
               <c:f>noise_event_rate_simulation!$D$2:$D$57</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>7.8433044276613986</c:v>
+                  <c:v>4.8433044276613986</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4921664938940777</c:v>
+                  <c:v>3.4921664938940782</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8817069765316843</c:v>
+                  <c:v>2.8817069765316843</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2883722060802265</c:v>
+                  <c:v>2.2883722060802265</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9434203134714485</c:v>
+                  <c:v>1.9434203134714481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6868149545073168</c:v>
+                  <c:v>1.686814954507317</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.4855723782917849</c:v>
+                  <c:v>1.4855723782917847</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3239015087485964</c:v>
+                  <c:v>1.3239015087485959</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1885066338181138</c:v>
+                  <c:v>1.1885066338181143</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.069908483023144</c:v>
+                  <c:v>1.0699084830231442</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9672670915597856</c:v>
+                  <c:v>0.96726709155978563</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8532265576830125</c:v>
+                  <c:v>0.8532265576830127</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.7672226754788052</c:v>
+                  <c:v>0.76722267547880518</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.6851234364220966</c:v>
+                  <c:v>0.6851234364220965</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6095197084184969</c:v>
+                  <c:v>0.60951970841849668</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5380644965213417</c:v>
+                  <c:v>0.53806449652134147</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4692253715261741</c:v>
+                  <c:v>0.46922537152617416</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4064635334680999</c:v>
+                  <c:v>0.40646353346809988</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3446378459177795</c:v>
+                  <c:v>0.34463784591777957</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.285681054052735</c:v>
+                  <c:v>0.28568105405273514</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2253092817258628</c:v>
+                  <c:v>0.22530928172586284</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.1650958747542179</c:v>
+                  <c:v>0.16509587475421802</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.1063099123315285</c:v>
+                  <c:v>0.10630991233152844</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.0470021305185053</c:v>
+                  <c:v>4.7002130518505408E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.9846398102960867</c:v>
+                  <c:v>-1.5360189703913245E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.9249766990651977</c:v>
+                  <c:v>-7.5023300934802029E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.8570006169263591</c:v>
+                  <c:v>-0.14299938307364082</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.7881330037009509</c:v>
+                  <c:v>-0.2118669962990492</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7145812088395314</c:v>
+                  <c:v>-0.28541879116046881</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.6454713949056066</c:v>
+                  <c:v>-0.3545286050943936</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.5625902246063346</c:v>
+                  <c:v>-0.4374097753936656</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.453407024934982</c:v>
+                  <c:v>-0.54659297506501814</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3704760795442938</c:v>
+                  <c:v>-0.62952392045570593</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.2796030725163301</c:v>
+                  <c:v>-0.72039692748366979</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.1826428681423296</c:v>
+                  <c:v>-0.81735713185767045</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0833879394805375</c:v>
+                  <c:v>-0.91661206051946242</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.9821173931664751</c:v>
+                  <c:v>-1.0178826068335249</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.8749570202063606</c:v>
+                  <c:v>-1.1250429797936394</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7652661058770105</c:v>
+                  <c:v>-1.2347338941229895</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.6500548398717485</c:v>
+                  <c:v>-1.3499451601282515</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.5301228251199708</c:v>
+                  <c:v>-1.469877174880029</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.4072889055313884</c:v>
+                  <c:v>-1.5927110944686116</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.2805328444513824</c:v>
+                  <c:v>-1.7194671555486176</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.1479235389806064</c:v>
+                  <c:v>-1.8520764610193936</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0155274043137872</c:v>
+                  <c:v>-1.9844725956862128</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.88524810778138618</c:v>
+                  <c:v>-2.1147518922186137</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.73925580326851059</c:v>
+                  <c:v>-2.2607441967314892</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.59461350916009803</c:v>
+                  <c:v>-2.4053864908399021</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.43584436598444132</c:v>
+                  <c:v>-2.5641556340155587</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.27044590801796259</c:v>
+                  <c:v>-2.7295540919820374</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.13481437032046015</c:v>
+                  <c:v>-2.8651856296795399</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-2.512002699306953E-2</c:v>
+                  <c:v>-3.0251200269930694</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.88074411072206338</c:v>
+                  <c:v>-3.8807441107220635</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-1.8013429130455774</c:v>
+                  <c:v>-4.8013429130455769</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-1.8597673278672833</c:v>
+                  <c:v>-4.8597673278672833</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-3.8649901774709172</c:v>
+                  <c:v>-6.8649901774709177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1153,7 +1253,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log10(thr/Vn)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1215,7 +1370,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log10(Rn/f3dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1474,106 +1684,106 @@
             <c:numRef>
               <c:f>noise_event_rate_simulation!$E$2:$E$57</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="56"/>
-                <c:pt idx="23">
-                  <c:v>3.0470021305185053</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.9846398102960867</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.9249766990651977</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.8570006169263591</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.7881330037009509</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.7145812088395314</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.6454713949056066</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.5625902246063346</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.453407024934982</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.3704760795442938</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2.2796030725163301</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.1826428681423296</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.0833879394805375</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.9821173931664751</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.8749570202063606</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.7652661058770105</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.6500548398717485</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.5301228251199708</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.4072889055313884</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.2805328444513824</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.1479235389806064</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.0155274043137872</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.88524810778138618</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.73925580326851059</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.59461350916009803</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.43584436598444132</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.27044590801796259</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.13481437032046015</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-2.512002699306953E-2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-0.88074411072206338</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-1.8013429130455774</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-1.8597673278672833</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-3.8649901774709172</c:v>
+                <c:pt idx="23" formatCode="0.000">
+                  <c:v>4.7002130518505408E-2</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.000">
+                  <c:v>-1.5360189703913245E-2</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.000">
+                  <c:v>-7.5023300934802029E-2</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.000">
+                  <c:v>-0.14299938307364082</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.000">
+                  <c:v>-0.2118669962990492</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.000">
+                  <c:v>-0.28541879116046881</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.000">
+                  <c:v>-0.3545286050943936</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.000">
+                  <c:v>-0.4374097753936656</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.000">
+                  <c:v>-0.54659297506501814</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.000">
+                  <c:v>-0.62952392045570593</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.000">
+                  <c:v>-0.72039692748366979</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.000">
+                  <c:v>-0.81735713185767045</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.000">
+                  <c:v>-0.91661206051946242</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.000">
+                  <c:v>-1.0178826068335249</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.000">
+                  <c:v>-1.1250429797936394</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.000">
+                  <c:v>-1.2347338941229895</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.000">
+                  <c:v>-1.3499451601282515</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.000">
+                  <c:v>-1.469877174880029</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.000">
+                  <c:v>-1.5927110944686116</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.000">
+                  <c:v>-1.7194671555486176</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.000">
+                  <c:v>-1.8520764610193936</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.000">
+                  <c:v>-1.9844725956862128</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.000">
+                  <c:v>-2.1147518922186137</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.000">
+                  <c:v>-2.2607441967314892</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.000">
+                  <c:v>-2.4053864908399021</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.000">
+                  <c:v>-2.5641556340155587</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.000">
+                  <c:v>-2.7295540919820374</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.000">
+                  <c:v>-2.8651856296795399</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.000">
+                  <c:v>-3.0251200269930694</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.000">
+                  <c:v>-3.8807441107220635</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.000">
+                  <c:v>-4.8013429130455769</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0.000">
+                  <c:v>-4.8597673278672833</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0.000">
+                  <c:v>-6.8649901774709177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,105 +1792,105 @@
             <c:numRef>
               <c:f>noise_event_rate_simulation!$F$2:$F$57</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="56"/>
-                <c:pt idx="23">
+                <c:pt idx="23" formatCode="0.000">
                   <c:v>0.29022432320211894</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="24" formatCode="0.000">
                   <c:v>0.30932030275701522</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="25" formatCode="0.000">
                   <c:v>0.32741349878278858</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="26" formatCode="0.000">
                   <c:v>0.34523332192791856</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="27" formatCode="0.000">
                   <c:v>0.36369582259457195</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="28" formatCode="0.000">
                   <c:v>0.37823341938381622</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="29" formatCode="0.000">
                   <c:v>0.39402312900855241</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="30" formatCode="0.000">
                   <c:v>0.40917540462998542</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="31" formatCode="0.000">
                   <c:v>0.42483069383949379</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="32" formatCode="0.000">
                   <c:v>0.43877549204844762</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="33" formatCode="0.000">
                   <c:v>0.45241823484386934</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="34" formatCode="0.000">
                   <c:v>0.46600855794598856</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="35" formatCode="0.000">
                   <c:v>0.4789718883173652</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="36" formatCode="0.000">
                   <c:v>0.49162051224656228</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="37" formatCode="0.000">
                   <c:v>0.50409825610187864</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="38" formatCode="0.000">
                   <c:v>0.51544900720562237</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="39" formatCode="0.000">
                   <c:v>0.52716107380393251</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="40" formatCode="0.000">
                   <c:v>0.53856468591090012</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="41" formatCode="0.000">
                   <c:v>0.54957838258145775</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="42" formatCode="0.000">
                   <c:v>0.56057597529491876</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="43" formatCode="0.000">
                   <c:v>0.57059547232740682</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="44" formatCode="0.000">
                   <c:v>0.58105900494217133</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="45" formatCode="0.000">
                   <c:v>0.59094031420585658</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="46" formatCode="0.000">
                   <c:v>0.60070777541602005</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="47" formatCode="0.000">
                   <c:v>0.61033165689837166</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="48" formatCode="0.000">
                   <c:v>0.61969257746878792</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="49" formatCode="0.000">
                   <c:v>0.6292018832728894</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="50" formatCode="0.000">
                   <c:v>0.63731317393678577</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="51" formatCode="0.000">
                   <c:v>0.64648155893638037</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="52" formatCode="0.000">
                   <c:v>0.68796107874421863</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="53" formatCode="0.000">
                   <c:v>0.72574114641589083</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="54" formatCode="0.000">
                   <c:v>0.72576148086188685</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="55" formatCode="0.000">
                   <c:v>0.7926279654693057</c:v>
                 </c:pt>
               </c:numCache>
@@ -1725,7 +1935,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>log10(Rn/f3dB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CH">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1787,7 +2057,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>log10(thr/Vn)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CH">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2996,16 +3326,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>449036</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>233688</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159204</xdr:rowOff>
+      <xdr:rowOff>1835</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533637</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3032,16 +3362,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>421820</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>291072</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>176891</xdr:rowOff>
+      <xdr:rowOff>162100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3365,1138 +3695,1569 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U54" sqref="U54"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>8.2179999999999996E-3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>69711500</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <f>LOG10(A2)</f>
         <v>-2.0852338630741474</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:E57" si="0">LOG10(B2)</f>
-        <v>7.8433044276613986</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2" s="4">
+        <f>LOG10(B2/1000)</f>
+        <v>4.8433044276613986</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>4.5401999999999998E-2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>3105750</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C57" si="1">LOG10(A3)</f>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C57" si="0">LOG10(A3)</f>
         <v>-1.3429250156487893</v>
       </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>6.4921664938940777</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D57" si="1">LOG10(B3/1000)</f>
+        <v>3.4921664938940782</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>8.5973999999999995E-2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>761565</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
         <v>-1.0656328669395938</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>5.8817069765316843</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8817069765316843</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>0.17632800000000001</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>194255</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
         <v>-0.75367871844401735</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>5.2883722060802265</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>2.2883722060802265</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>0.27147100000000002</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>87785</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
         <v>-0.56627655728198378</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>4.9434203134714485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9434203134714481</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>0.361294</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>48620</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
         <v>-0.44213925068918297</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>4.6868149545073168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>1.686814954507317</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>0.438523</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>30589.5</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
         <v>-0.35800762348122533</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>4.4855723782917849</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>1.4855723782917847</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>0.52510900000000005</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>21081.5</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
         <v>-0.27975053814630579</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>4.3239015087485964</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3239015087485959</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>0.62245600000000001</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>15435</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
         <v>-0.20589134243716131</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>4.1885066338181138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1885066338181143</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>0.70840000000000003</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>11746.5</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
         <v>-0.14972144748196284</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>4.069908483023144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0699084830231442</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>0.79827599999999999</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>9274</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
         <v>-9.7846927504907366E-2</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>3.9672670915597856</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.96726709155978563</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>0.88257200000000002</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>7132.25</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
         <v>-5.4249854861164702E-2</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>3.8532265576830125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8532265576830127</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>0.97673900000000002</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>5850.9</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
         <v>-1.0221471084699691E-2</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>3.7672226754788052</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.76722267547880518</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>1.0635699999999999</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>4843.1000000000004</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
         <v>2.6766078736431605E-2</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>3.6851234364220966</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6851234364220965</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>1.1469100000000001</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>4069.3</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
         <v>5.9529339403513792E-2</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>3.6095197084184969</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60951970841849668</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>1.2392289999999999</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>3451.95</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
         <v>9.315156807636546E-2</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>3.5380644965213417</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.53806449652134147</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>1.3280240000000001</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>2945.95</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
         <v>0.12320592365653371</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>3.4692253715261741</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.46922537152617416</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>1.4188210000000001</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>2549.5500000000002</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
         <v>0.15192760784940165</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>3.4064635334680999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40646353346809988</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>1.5046569999999999</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>2211.25</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
         <v>0.17743750990678792</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>3.3446378459177795</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.34463784591777957</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>1.5957159999999999</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>1930.55</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
         <v>0.20295559966634624</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>3.285681054052735</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="D21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28568105405273514</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>1.6896260000000001</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>1680</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
         <v>0.22779058383764991</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>3.2253092817258628</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="D22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22530928172586284</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>1.771684</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>1462.5</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
         <v>0.24838626309592524</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>3.1650958747542179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16509587475421802</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>1.8610279999999999</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>1277.3499999999999</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
         <v>0.26975290733496615</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>3.1063099123315285</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="D24" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10630991233152844</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>1.950852</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>1114.3</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
         <v>0.29022432320211894</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>3.0470021305185053</v>
-      </c>
-      <c r="E25">
-        <v>3.0470021305185053</v>
-      </c>
-      <c r="F25">
+      <c r="D25" s="4">
+        <f t="shared" si="1"/>
+        <v>4.7002130518505408E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4.7002130518505408E-2</v>
+      </c>
+      <c r="F25" s="2">
         <v>0.29022432320211894</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="G25" s="3">
+        <f>10^F25</f>
+        <v>1.950852</v>
+      </c>
+      <c r="H25" s="2">
+        <f>1/G25</f>
+        <v>0.51259654755973283</v>
+      </c>
+      <c r="I25" s="2">
+        <f>0.2*H25</f>
+        <v>0.10251930951194657</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>2.0385450000000001</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>965.25</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
         <v>0.30932030275701522</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>2.9846398102960867</v>
-      </c>
-      <c r="E26">
-        <v>2.9846398102960867</v>
-      </c>
-      <c r="F26">
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.5360189703913245E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>-1.5360189703913245E-2</v>
+      </c>
+      <c r="F26" s="2">
         <v>0.30932030275701522</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="G26" s="3">
+        <f t="shared" ref="G26:G57" si="2">10^F26</f>
+        <v>2.0385450000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" ref="H26:H57" si="3">1/G26</f>
+        <v>0.49054595311852323</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" ref="I26:I57" si="4">0.2*H26</f>
+        <v>9.8109190623704656E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>2.125267</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>841.35</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
         <v>0.32741349878278858</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>2.9249766990651977</v>
-      </c>
-      <c r="E27">
-        <v>2.9249766990651977</v>
-      </c>
-      <c r="F27">
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>-7.5023300934802029E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-7.5023300934802029E-2</v>
+      </c>
+      <c r="F27" s="2">
         <v>0.32741349878278858</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="G27" s="3">
+        <f t="shared" si="2"/>
+        <v>2.125267</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.47052911469476538</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="4"/>
+        <v>9.4105822938953088E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>2.2142840000000001</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>719.45</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
         <v>0.34523332192791856</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>2.8570006169263591</v>
-      </c>
-      <c r="E28">
-        <v>2.8570006169263591</v>
-      </c>
-      <c r="F28">
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.14299938307364082</v>
+      </c>
+      <c r="E28" s="2">
+        <v>-0.14299938307364082</v>
+      </c>
+      <c r="F28" s="2">
         <v>0.34523332192791856</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="G28" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2142840000000006</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
+        <v>0.45161325286187304</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="4"/>
+        <v>9.032265057237461E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>2.3104460000000002</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>613.95000000000005</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
         <v>0.36369582259457195</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>2.7881330037009509</v>
-      </c>
-      <c r="E29">
-        <v>2.7881330037009509</v>
-      </c>
-      <c r="F29">
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.2118669962990492</v>
+      </c>
+      <c r="E29" s="2">
+        <v>-0.2118669962990492</v>
+      </c>
+      <c r="F29" s="2">
         <v>0.36369582259457195</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="G29" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3104460000000002</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="3"/>
+        <v>0.43281686739270248</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="4"/>
+        <v>8.6563373478540498E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>2.3890950000000002</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>518.29999999999995</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
         <v>0.37823341938381622</v>
       </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>2.7145812088395314</v>
-      </c>
-      <c r="E30">
-        <v>2.7145812088395314</v>
-      </c>
-      <c r="F30">
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.28541879116046881</v>
+      </c>
+      <c r="E30" s="2">
+        <v>-0.28541879116046881</v>
+      </c>
+      <c r="F30" s="2">
         <v>0.37823341938381622</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="G30" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3890950000000002</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="3"/>
+        <v>0.41856853745874478</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="4"/>
+        <v>8.3713707491748959E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>2.477554</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>442.05</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
         <v>0.39402312900855241</v>
       </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>2.6454713949056066</v>
-      </c>
-      <c r="E31">
-        <v>2.6454713949056066</v>
-      </c>
-      <c r="F31">
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.3545286050943936</v>
+      </c>
+      <c r="E31" s="2">
+        <v>-0.3545286050943936</v>
+      </c>
+      <c r="F31" s="2">
         <v>0.39402312900855241</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="G31" s="3">
+        <f t="shared" si="2"/>
+        <v>2.4775540000000005</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="3"/>
+        <v>0.40362389679498401</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="4"/>
+        <v>8.0724779358996801E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>2.5655199999999998</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>365.25</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
         <v>0.40917540462998542</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>2.5625902246063346</v>
-      </c>
-      <c r="E32">
-        <v>2.5625902246063346</v>
-      </c>
-      <c r="F32">
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.4374097753936656</v>
+      </c>
+      <c r="E32" s="2">
+        <v>-0.4374097753936656</v>
+      </c>
+      <c r="F32" s="2">
         <v>0.40917540462998542</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="G32" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5655200000000002</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="3"/>
+        <v>0.38978452711341166</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="4"/>
+        <v>7.795690542268234E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>2.6596880000000001</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>284.05799999999999</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="1"/>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
         <v>0.42483069383949379</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>2.453407024934982</v>
-      </c>
-      <c r="E33">
-        <v>2.453407024934982</v>
-      </c>
-      <c r="F33">
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.54659297506501814</v>
+      </c>
+      <c r="E33" s="2">
+        <v>-0.54659297506501814</v>
+      </c>
+      <c r="F33" s="2">
         <v>0.42483069383949379</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="G33" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6596880000000001</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="3"/>
+        <v>0.37598394999714252</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="4"/>
+        <v>7.5196789999428512E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>2.7464740000000001</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>234.68</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="1"/>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
         <v>0.43877549204844762</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>2.3704760795442938</v>
-      </c>
-      <c r="E34">
-        <v>2.3704760795442938</v>
-      </c>
-      <c r="F34">
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.62952392045570593</v>
+      </c>
+      <c r="E34" s="2">
+        <v>-0.62952392045570593</v>
+      </c>
+      <c r="F34" s="2">
         <v>0.43877549204844762</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="G34" s="3">
+        <f t="shared" si="2"/>
+        <v>2.7464740000000005</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.36410321015236258</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="4"/>
+        <v>7.2820642030472518E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>2.83412</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>190.37200000000001</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="1"/>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
         <v>0.45241823484386934</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>2.2796030725163301</v>
-      </c>
-      <c r="E35">
-        <v>2.2796030725163301</v>
-      </c>
-      <c r="F35">
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.72039692748366979</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-0.72039692748366979</v>
+      </c>
+      <c r="F35" s="2">
         <v>0.45241823484386934</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="G35" s="3">
+        <f t="shared" si="2"/>
+        <v>2.83412</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35284321059094181</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="4"/>
+        <v>7.0568642118188363E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>2.92421</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>152.28</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="1"/>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
         <v>0.46600855794598856</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>2.1826428681423296</v>
-      </c>
-      <c r="E36">
-        <v>2.1826428681423296</v>
-      </c>
-      <c r="F36">
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.81735713185767045</v>
+      </c>
+      <c r="E36" s="2">
+        <v>-0.81735713185767045</v>
+      </c>
+      <c r="F36" s="2">
         <v>0.46600855794598856</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="G36" s="3">
+        <f t="shared" si="2"/>
+        <v>2.9242100000000004</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="3"/>
+        <v>0.34197270373878752</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="4"/>
+        <v>6.8394540747757512E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>3.0128110000000001</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>121.16800000000001</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="1"/>
+      <c r="C37" s="4">
+        <f t="shared" si="0"/>
         <v>0.4789718883173652</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>2.0833879394805375</v>
-      </c>
-      <c r="E37">
-        <v>2.0833879394805375</v>
-      </c>
-      <c r="F37">
+      <c r="D37" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.91661206051946242</v>
+      </c>
+      <c r="E37" s="2">
+        <v>-0.91661206051946242</v>
+      </c>
+      <c r="F37" s="2">
         <v>0.4789718883173652</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="G37" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0128110000000006</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="3"/>
+        <v>0.33191594162395177</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="4"/>
+        <v>6.6383188324790357E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>3.1018479999999999</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>95.965999999999994</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="1"/>
+      <c r="C38" s="4">
+        <f t="shared" si="0"/>
         <v>0.49162051224656228</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>1.9821173931664751</v>
-      </c>
-      <c r="E38">
-        <v>1.9821173931664751</v>
-      </c>
-      <c r="F38">
+      <c r="D38" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.0178826068335249</v>
+      </c>
+      <c r="E38" s="2">
+        <v>-1.0178826068335249</v>
+      </c>
+      <c r="F38" s="2">
         <v>0.49162051224656228</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="G38" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1018480000000008</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="3"/>
+        <v>0.32238846004059507</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="4"/>
+        <v>6.4477692008119022E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
         <v>3.1922600000000001</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="5">
         <v>74.981999999999999</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="1"/>
+      <c r="C39" s="5">
+        <f t="shared" si="0"/>
         <v>0.50409825610187864</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>1.8749570202063606</v>
-      </c>
-      <c r="E39">
-        <v>1.8749570202063606</v>
-      </c>
-      <c r="F39">
+      <c r="D39" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.1250429797936394</v>
+      </c>
+      <c r="E39" s="5">
+        <v>-1.1250429797936394</v>
+      </c>
+      <c r="F39" s="5">
         <v>0.50409825610187864</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="G39" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1922600000000005</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="3"/>
+        <v>0.31325769204262804</v>
+      </c>
+      <c r="I39" s="5">
+        <f t="shared" si="4"/>
+        <v>6.2651538408525609E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>3.2767930000000001</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>58.246000000000002</v>
       </c>
-      <c r="C40">
-        <f t="shared" si="1"/>
+      <c r="C40" s="4">
+        <f t="shared" si="0"/>
         <v>0.51544900720562237</v>
       </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>1.7652661058770105</v>
-      </c>
-      <c r="E40">
-        <v>1.7652661058770105</v>
-      </c>
-      <c r="F40">
+      <c r="D40" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.2347338941229895</v>
+      </c>
+      <c r="E40" s="2">
+        <v>-1.2347338941229895</v>
+      </c>
+      <c r="F40" s="2">
         <v>0.51544900720562237</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="G40" s="3">
+        <f t="shared" si="2"/>
+        <v>3.276793000000001</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="3"/>
+        <v>0.30517643317719478</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="4"/>
+        <v>6.1035286635438959E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>3.3663639999999999</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>44.673999999999999</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="1"/>
+      <c r="C41" s="4">
+        <f t="shared" si="0"/>
         <v>0.52716107380393251</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="0"/>
-        <v>1.6500548398717485</v>
-      </c>
-      <c r="E41">
-        <v>1.6500548398717485</v>
-      </c>
-      <c r="F41">
+      <c r="D41" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.3499451601282515</v>
+      </c>
+      <c r="E41" s="2">
+        <v>-1.3499451601282515</v>
+      </c>
+      <c r="F41" s="2">
         <v>0.52716107380393251</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="G41" s="3">
+        <f t="shared" si="2"/>
+        <v>3.3663640000000008</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="3"/>
+        <v>0.29705640863554855</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="4"/>
+        <v>5.9411281727109716E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>3.4559280000000001</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>33.893999999999998</v>
       </c>
-      <c r="C42">
-        <f t="shared" si="1"/>
+      <c r="C42" s="4">
+        <f t="shared" si="0"/>
         <v>0.53856468591090012</v>
       </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
-        <v>1.5301228251199708</v>
-      </c>
-      <c r="E42">
-        <v>1.5301228251199708</v>
-      </c>
-      <c r="F42">
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.469877174880029</v>
+      </c>
+      <c r="E42" s="2">
+        <v>-1.469877174880029</v>
+      </c>
+      <c r="F42" s="2">
         <v>0.53856468591090012</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="G42" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4559280000000001</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="3"/>
+        <v>0.28935788014102143</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="4"/>
+        <v>5.7871576028204287E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>3.5446909999999998</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>25.544</v>
       </c>
-      <c r="C43">
-        <f t="shared" si="1"/>
+      <c r="C43" s="4">
+        <f t="shared" si="0"/>
         <v>0.54957838258145775</v>
       </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>1.4072889055313884</v>
-      </c>
-      <c r="E43">
-        <v>1.4072889055313884</v>
-      </c>
-      <c r="F43">
+      <c r="D43" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.5927110944686116</v>
+      </c>
+      <c r="E43" s="2">
+        <v>-1.5927110944686116</v>
+      </c>
+      <c r="F43" s="2">
         <v>0.54957838258145775</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="G43" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5446910000000007</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="3"/>
+        <v>0.28211203741031299</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="4"/>
+        <v>5.6422407482062599E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>3.635599</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>19.077999999999999</v>
       </c>
-      <c r="C44">
-        <f t="shared" si="1"/>
+      <c r="C44" s="4">
+        <f t="shared" si="0"/>
         <v>0.56057597529491876</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>1.2805328444513824</v>
-      </c>
-      <c r="E44">
-        <v>1.2805328444513824</v>
-      </c>
-      <c r="F44">
+      <c r="D44" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.7194671555486176</v>
+      </c>
+      <c r="E44" s="2">
+        <v>-1.7194671555486176</v>
+      </c>
+      <c r="F44" s="2">
         <v>0.56057597529491876</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="G44" s="3">
+        <f t="shared" si="2"/>
+        <v>3.6355990000000009</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27505783778684056</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="4"/>
+        <v>5.5011567557368114E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>3.72045</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>14.058</v>
       </c>
-      <c r="C45">
-        <f t="shared" si="1"/>
+      <c r="C45" s="4">
+        <f t="shared" si="0"/>
         <v>0.57059547232740682</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>1.1479235389806064</v>
-      </c>
-      <c r="E45">
-        <v>1.1479235389806064</v>
-      </c>
-      <c r="F45">
+      <c r="D45" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.8520764610193936</v>
+      </c>
+      <c r="E45" s="2">
+        <v>-1.8520764610193936</v>
+      </c>
+      <c r="F45" s="2">
         <v>0.57059547232740682</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="G45" s="3">
+        <f t="shared" si="2"/>
+        <v>3.7204500000000005</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26878469002405619</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="4"/>
+        <v>5.3756938004811239E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>3.8111760000000001</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>10.364000000000001</v>
       </c>
-      <c r="C46">
-        <f t="shared" si="1"/>
+      <c r="C46" s="4">
+        <f t="shared" si="0"/>
         <v>0.58105900494217133</v>
       </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
-        <v>1.0155274043137872</v>
-      </c>
-      <c r="E46">
-        <v>1.0155274043137872</v>
-      </c>
-      <c r="F46">
+      <c r="D46" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9844725956862128</v>
+      </c>
+      <c r="E46" s="2">
+        <v>-1.9844725956862128</v>
+      </c>
+      <c r="F46" s="2">
         <v>0.58105900494217133</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="G46" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8111760000000006</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26238620310371386</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2477240620742771E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>3.8988839999999998</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>7.6779999999999999</v>
       </c>
-      <c r="C47">
-        <f t="shared" si="1"/>
+      <c r="C47" s="4">
+        <f t="shared" si="0"/>
         <v>0.59094031420585658</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="0"/>
-        <v>0.88524810778138618</v>
-      </c>
-      <c r="E47">
-        <v>0.88524810778138618</v>
-      </c>
-      <c r="F47">
+      <c r="D47" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1147518922186137</v>
+      </c>
+      <c r="E47" s="2">
+        <v>-2.1147518922186137</v>
+      </c>
+      <c r="F47" s="2">
         <v>0.59094031420585658</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="G47" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8988840000000007</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25648365019323471</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1296730038646945E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>3.987565</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>5.4859999999999998</v>
       </c>
-      <c r="C48">
-        <f t="shared" si="1"/>
+      <c r="C48" s="4">
+        <f t="shared" si="0"/>
         <v>0.60070777541602005</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="0"/>
-        <v>0.73925580326851059</v>
-      </c>
-      <c r="E48">
-        <v>0.73925580326851059</v>
-      </c>
-      <c r="F48">
+      <c r="D48" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.2607441967314892</v>
+      </c>
+      <c r="E48" s="2">
+        <v>-2.2607441967314892</v>
+      </c>
+      <c r="F48" s="2">
         <v>0.60070777541602005</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="G48" s="3">
+        <f t="shared" si="2"/>
+        <v>3.987565</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25077961111605707</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="4"/>
+        <v>5.0155922223211413E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>4.0769149999999996</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>3.9319999999999999</v>
       </c>
-      <c r="C49">
-        <f t="shared" si="1"/>
+      <c r="C49" s="4">
+        <f t="shared" si="0"/>
         <v>0.61033165689837166</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="0"/>
-        <v>0.59461350916009803</v>
-      </c>
-      <c r="E49">
-        <v>0.59461350916009803</v>
-      </c>
-      <c r="F49">
+      <c r="D49" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.4053864908399021</v>
+      </c>
+      <c r="E49" s="2">
+        <v>-2.4053864908399021</v>
+      </c>
+      <c r="F49" s="2">
         <v>0.61033165689837166</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="G49" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0769150000000005</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24528350480694344</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="4"/>
+        <v>4.9056700961388693E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>4.1657440000000001</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>2.7280000000000002</v>
       </c>
-      <c r="C50">
-        <f t="shared" si="1"/>
+      <c r="C50" s="4">
+        <f t="shared" si="0"/>
         <v>0.61969257746878792</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="0"/>
-        <v>0.43584436598444132</v>
-      </c>
-      <c r="E50">
-        <v>0.43584436598444132</v>
-      </c>
-      <c r="F50">
+      <c r="D50" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.5641556340155587</v>
+      </c>
+      <c r="E50" s="2">
+        <v>-2.5641556340155587</v>
+      </c>
+      <c r="F50" s="2">
         <v>0.61969257746878792</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="G50" s="3">
+        <f t="shared" si="2"/>
+        <v>4.1657440000000001</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24005315737116825</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="4"/>
+        <v>4.801063147423365E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>4.2579630000000002</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>1.8640000000000001</v>
       </c>
-      <c r="C51">
-        <f t="shared" si="1"/>
+      <c r="C51" s="4">
+        <f t="shared" si="0"/>
         <v>0.6292018832728894</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="0"/>
-        <v>0.27044590801796259</v>
-      </c>
-      <c r="E51">
-        <v>0.27044590801796259</v>
-      </c>
-      <c r="F51">
+      <c r="D51" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.7295540919820374</v>
+      </c>
+      <c r="E51" s="2">
+        <v>-2.7295540919820374</v>
+      </c>
+      <c r="F51" s="2">
         <v>0.6292018832728894</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="G51" s="3">
+        <f t="shared" si="2"/>
+        <v>4.2579630000000002</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="3"/>
+        <v>0.23485408398335073</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6970816796670145E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>4.3382360000000002</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>1.3640000000000001</v>
       </c>
-      <c r="C52">
-        <f t="shared" si="1"/>
+      <c r="C52" s="4">
+        <f t="shared" si="0"/>
         <v>0.63731317393678577</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="0"/>
-        <v>0.13481437032046015</v>
-      </c>
-      <c r="E52">
-        <v>0.13481437032046015</v>
-      </c>
-      <c r="F52">
+      <c r="D52" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.8651856296795399</v>
+      </c>
+      <c r="E52" s="2">
+        <v>-2.8651856296795399</v>
+      </c>
+      <c r="F52" s="2">
         <v>0.63731317393678577</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="G52" s="3">
+        <f t="shared" si="2"/>
+        <v>4.3382360000000002</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="3"/>
+        <v>0.23050843706981361</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6101687413962728E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>4.4307939999999997</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>0.94379999999999997</v>
       </c>
-      <c r="C53">
-        <f t="shared" si="1"/>
+      <c r="C53" s="4">
+        <f t="shared" si="0"/>
         <v>0.64648155893638037</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="0"/>
-        <v>-2.512002699306953E-2</v>
-      </c>
-      <c r="E53">
-        <v>-2.512002699306953E-2</v>
-      </c>
-      <c r="F53">
+      <c r="D53" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.0251200269930694</v>
+      </c>
+      <c r="E53" s="2">
+        <v>-3.0251200269930694</v>
+      </c>
+      <c r="F53" s="2">
         <v>0.64648155893638037</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="G53" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4307940000000006</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22569318275686026</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="4"/>
+        <v>4.5138636551372055E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>4.8748480000000001</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>0.13159999999999999</v>
       </c>
-      <c r="C54">
-        <f t="shared" si="1"/>
+      <c r="C54" s="4">
+        <f t="shared" si="0"/>
         <v>0.68796107874421863</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="0"/>
-        <v>-0.88074411072206338</v>
-      </c>
-      <c r="E54">
-        <v>-0.88074411072206338</v>
-      </c>
-      <c r="F54">
+      <c r="D54" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.8807441107220635</v>
+      </c>
+      <c r="E54" s="2">
+        <v>-3.8807441107220635</v>
+      </c>
+      <c r="F54" s="2">
         <v>0.68796107874421863</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="G54" s="3">
+        <f t="shared" si="2"/>
+        <v>4.874848000000001</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="3"/>
+        <v>0.20513460111987078</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="4"/>
+        <v>4.102692022397416E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>5.3179119999999998</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="C55">
-        <f t="shared" si="1"/>
+      <c r="C55" s="4">
+        <f t="shared" si="0"/>
         <v>0.72574114641589083</v>
       </c>
-      <c r="D55">
-        <f t="shared" si="0"/>
-        <v>-1.8013429130455774</v>
-      </c>
-      <c r="E55">
-        <v>-1.8013429130455774</v>
-      </c>
-      <c r="F55">
+      <c r="D55" s="4">
+        <f t="shared" si="1"/>
+        <v>-4.8013429130455769</v>
+      </c>
+      <c r="E55" s="2">
+        <v>-4.8013429130455769</v>
+      </c>
+      <c r="F55" s="2">
         <v>0.72574114641589083</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="G55" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3179119999999998</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18804372844078654</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="4"/>
+        <v>3.7608745688157308E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>5.3181609999999999</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>1.3811240000000001E-2</v>
       </c>
-      <c r="C56">
-        <f t="shared" si="1"/>
+      <c r="C56" s="4">
+        <f t="shared" si="0"/>
         <v>0.72576148086188685</v>
       </c>
-      <c r="D56">
-        <f t="shared" si="0"/>
-        <v>-1.8597673278672833</v>
-      </c>
-      <c r="E56">
-        <v>-1.8597673278672833</v>
-      </c>
-      <c r="F56">
+      <c r="D56" s="4">
+        <f t="shared" si="1"/>
+        <v>-4.8597673278672833</v>
+      </c>
+      <c r="E56" s="2">
+        <v>-4.8597673278672833</v>
+      </c>
+      <c r="F56" s="2">
         <v>0.72576148086188685</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="G56" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3181610000000008</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18803492410252337</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="4"/>
+        <v>3.7606984820504674E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>6.2033740000000002</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>1.3646139999999999E-4</v>
       </c>
-      <c r="C57">
-        <f t="shared" si="1"/>
+      <c r="C57" s="4">
+        <f t="shared" si="0"/>
         <v>0.7926279654693057</v>
       </c>
-      <c r="D57">
-        <f t="shared" si="0"/>
-        <v>-3.8649901774709172</v>
-      </c>
-      <c r="E57">
-        <v>-3.8649901774709172</v>
-      </c>
-      <c r="F57">
+      <c r="D57" s="4">
+        <f t="shared" si="1"/>
+        <v>-6.8649901774709177</v>
+      </c>
+      <c r="E57" s="2">
+        <v>-6.8649901774709177</v>
+      </c>
+      <c r="F57" s="2">
         <v>0.7926279654693057</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="2"/>
+        <v>6.2033740000000019</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="3"/>
+        <v>0.16120259716728344</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="4"/>
+        <v>3.2240519433456689E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added fig. 3 to spreadsheet
</commit_message>
<xml_diff>
--- a/media/noise_event_rate_simulation.xlsx
+++ b/media/noise_event_rate_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tobi\Dropbox (Personal)\GitHub\SensorsINI\v2e\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1E474E-F736-4831-9243-C3A028AC1A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623F5263-7962-4421-9A45-C450824DA3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4950" yWindow="720" windowWidth="37890" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3396,6 +3396,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1350064</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>91109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>463407</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>91469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D55EB1-9ADB-F3CD-1135-CE7D25AEE64D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095499" y="9235109"/>
+          <a:ext cx="6079017" cy="4381860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3700,7 +3744,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
--photoreceptor_noise temporal simulation of shot noise is working now given sufficiently high (10X higher) sample rate than --cutoff_freq_hz
</commit_message>
<xml_diff>
--- a/media/noise_event_rate_simulation.xlsx
+++ b/media/noise_event_rate_simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tobi\Dropbox (Personal)\GitHub\SensorsINI\v2e\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623F5263-7962-4421-9A45-C450824DA3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058EE178-1D5E-4E4E-BFC5-675656F875B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="720" windowWidth="37890" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35235" yWindow="3120" windowWidth="36645" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="noise_event_rate_simulation" sheetId="1" r:id="rId1"/>
@@ -3742,9 +3742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>